<commit_message>
Interaction terms, updated feedback loop analysis, various other changes
</commit_message>
<xml_diff>
--- a/Examples/Kumu/Sleep.xlsx
+++ b/Examples/Kumu/Sleep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbw209/Library/Mobile Documents/com~apple~CloudDocs/Documents/KU/Coding/SDM package/connections/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbw209/Library/Mobile Documents/com~apple~CloudDocs/Documents/Research/systemdynamics/Examples/Kumu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DC1221-DEEB-E84A-9DD7-D4927DB8842F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B974949-4BF8-1F4C-A9A9-6AC1D0B97029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26520" yWindow="-1400" windowWidth="14400" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
@@ -473,9 +473,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -491,7 +497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -499,7 +505,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -507,7 +513,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -515,7 +521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -531,7 +537,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -544,10 +550,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="42" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -564,11 +570,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -869,7 +879,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -889,14 +899,14 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+      <c r="B2" t="s">
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Implement user changes in app
</commit_message>
<xml_diff>
--- a/Examples/Kumu/Sleep.xlsx
+++ b/Examples/Kumu/Sleep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbw209/Library/Mobile Documents/com~apple~CloudDocs/Documents/Research/systemdynamics/Examples/Kumu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B974949-4BF8-1F4C-A9A9-6AC1D0B97029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F609A5-1130-8443-ADFA-F9CE1B1BCFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26520" yWindow="-1400" windowWidth="14400" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -571,7 +571,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -603,7 +603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -617,7 +617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -631,7 +631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -645,7 +645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -673,7 +673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -687,7 +687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -701,7 +701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -715,7 +715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -729,7 +729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -743,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -757,7 +757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -771,7 +771,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -785,7 +785,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -799,7 +799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -813,7 +813,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -827,7 +827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -841,7 +841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -855,7 +855,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1081127A-7B42-0246-A96F-A7185E3DDBD3}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>